<commit_message>
Updates to code. Done through the latest round of single and mixed inoculation trials. Need to add older data.
</commit_message>
<xml_diff>
--- a/Final_CW_data_collection.xlsx
+++ b/Final_CW_data_collection.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jason\Dropbox\My PC (DESKTOP-IOO274E)\Desktop\Data\Lemna_singleinoculations\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jason\Dropbox\My PC (DESKTOP-IOO274E)\Desktop\Data\Lemna_singleinoculations\Lemna_single_inoculations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9E3186F-90AB-441A-9DCA-8150BF55FED4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F86C121B-B60A-4239-9557-D16DACBA0A9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15840" yWindow="255" windowWidth="12435" windowHeight="15315" xr2:uid="{95C0FB3A-527F-4951-96EE-3A6B4D5B4F0A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{95C0FB3A-527F-4951-96EE-3A6B4D5B4F0A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -487,8 +487,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81A44AB1-0B27-479B-B8F6-3223D40480CC}">
   <dimension ref="A1:O921"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H900" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L923" sqref="L923"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>